<commit_message>
// VJ made channel DX equal to DX, tried different channel 1D2D interaction, interface tweaks
</commit_message>
<xml_diff>
--- a/docs/interception.xlsx
+++ b/docs/interception.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18192" windowHeight="8508"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -94,7 +94,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -112,7 +112,7 @@
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="1"/>
           <c:order val="0"/>
           <c:marker>
             <c:symbol val="none"/>
@@ -167,7 +167,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$7:$E$19</c:f>
+              <c:f>Sheet1!$F$7:$F$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -175,40 +175,40 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.38644586837665329</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.6484413957654851</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>0.82606434891050351</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>0.94648592174572821</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>1.0281271451762939</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>1.0834767740368954</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>1.1210017067396962</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>1.1464421767724058</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>1.1636898430270317</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>1.175383101478958</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>1.183310683750378</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>1.1886852815092928</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -216,7 +216,7 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:ser>
-          <c:idx val="1"/>
+          <c:idx val="2"/>
           <c:order val="1"/>
           <c:marker>
             <c:symbol val="none"/>
@@ -271,7 +271,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$F$7:$F$19</c:f>
+              <c:f>Sheet1!$G$7:$G$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -279,40 +279,40 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.11916680215186558</c:v>
+                  <c:v>0.36064817401002547</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.16732997062822177</c:v>
+                  <c:v>0.59122924260328524</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.18679588526043345</c:v>
+                  <c:v>0.73865166984710562</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.19466334590423576</c:v>
+                  <c:v>0.83290646789731626</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.19784310591815016</c:v>
+                  <c:v>0.89316844513903471</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.19912825676972182</c:v>
+                  <c:v>0.93169705032629369</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.19964767103497078</c:v>
+                  <c:v>0.95633038440561458</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.19985760061531083</c:v>
+                  <c:v>0.97207975152944937</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.19994244701181985</c:v>
+                  <c:v>0.98214913815825966</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.19997673903959842</c:v>
+                  <c:v>0.98858701888598854</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.19999059871092861</c:v>
+                  <c:v>0.99270308968476773</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.19999620031870233</c:v>
+                  <c:v>0.99533470706587113</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -320,7 +320,7 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:ser>
-          <c:idx val="2"/>
+          <c:idx val="3"/>
           <c:order val="2"/>
           <c:marker>
             <c:symbol val="none"/>
@@ -375,7 +375,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$G$7:$G$19</c:f>
+              <c:f>Sheet1!$H$7:$H$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -383,40 +383,40 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.20949534655833113</c:v>
+                  <c:v>0.32518581747851849</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.30926994254267415</c:v>
+                  <c:v>0.51818936509557145</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.35678875461837362</c:v>
+                  <c:v>0.63274039220249267</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.37942014168447585</c:v>
+                  <c:v>0.7007284575684537</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.39019860305930609</c:v>
+                  <c:v>0.74108057966589846</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.39533197068142223</c:v>
+                  <c:v>0.76503027949928004</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.39777679673102195</c:v>
+                  <c:v>0.77924485093430751</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.39894117357928238</c:v>
+                  <c:v>0.78768145107907717</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.3994957215991658</c:v>
+                  <c:v>0.79268872283032643</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.39975983154502742</c:v>
+                  <c:v>0.79566062738436694</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.39988561697929459</c:v>
+                  <c:v>0.79742450542356513</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.39994552375570225</c:v>
+                  <c:v>0.79847139831012692</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -424,7 +424,7 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:ser>
-          <c:idx val="3"/>
+          <c:idx val="4"/>
           <c:order val="3"/>
           <c:marker>
             <c:symbol val="none"/>
@@ -479,7 +479,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$H$7:$H$19</c:f>
+              <c:f>Sheet1!$I$7:$I$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -528,7 +528,7 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:ser>
-          <c:idx val="4"/>
+          <c:idx val="5"/>
           <c:order val="4"/>
           <c:marker>
             <c:symbol val="none"/>
@@ -583,7 +583,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$I$7:$I$19</c:f>
+              <c:f>Sheet1!$J$7:$J$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -591,40 +591,40 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.32518581747851849</c:v>
+                  <c:v>0.20949534655833113</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.51818936509557145</c:v>
+                  <c:v>0.30926994254267415</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.63274039220249267</c:v>
+                  <c:v>0.35678875461837362</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.7007284575684537</c:v>
+                  <c:v>0.37942014168447585</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.74108057966589846</c:v>
+                  <c:v>0.39019860305930609</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.76503027949928004</c:v>
+                  <c:v>0.39533197068142223</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.77924485093430751</c:v>
+                  <c:v>0.39777679673102195</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.78768145107907717</c:v>
+                  <c:v>0.39894117357928238</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.79268872283032643</c:v>
+                  <c:v>0.3994957215991658</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.79566062738436694</c:v>
+                  <c:v>0.39975983154502742</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.79742450542356513</c:v>
+                  <c:v>0.39988561697929459</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.79847139831012692</c:v>
+                  <c:v>0.39994552375570225</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -632,7 +632,7 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:ser>
-          <c:idx val="5"/>
+          <c:idx val="6"/>
           <c:order val="5"/>
           <c:marker>
             <c:symbol val="none"/>
@@ -687,110 +687,6 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$J$7:$J$19</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.36064817401002547</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.59122924260328524</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.73865166984710562</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.83290646789731626</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.89316844513903471</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.93169705032629369</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.95633038440561458</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.97207975152944937</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.98214913815825966</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.98858701888598854</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.99270308968476773</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.99533470706587113</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="6"/>
-          <c:order val="6"/>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$D$7:$D$19</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.5</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2.5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>3.5</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>4.5</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>5.5</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>6</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
               <c:f>Sheet1!$K$7:$K$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
@@ -799,40 +695,40 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.38644586837665329</c:v>
+                  <c:v>0.11916680215186558</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.6484413957654851</c:v>
+                  <c:v>0.16732997062822177</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.82606434891050351</c:v>
+                  <c:v>0.18679588526043345</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.94648592174572821</c:v>
+                  <c:v>0.19466334590423576</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.0281271451762939</c:v>
+                  <c:v>0.19784310591815016</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.0834767740368954</c:v>
+                  <c:v>0.19912825676972182</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.1210017067396962</c:v>
+                  <c:v>0.19964767103497078</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.1464421767724058</c:v>
+                  <c:v>0.19985760061531083</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.1636898430270317</c:v>
+                  <c:v>0.19994244701181985</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.175383101478958</c:v>
+                  <c:v>0.19997673903959842</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.183310683750378</c:v>
+                  <c:v>0.19999059871092861</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.1886852815092928</c:v>
+                  <c:v>0.19999620031870233</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -847,11 +743,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="29345664"/>
-        <c:axId val="29347840"/>
+        <c:axId val="167627008"/>
+        <c:axId val="167776640"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="29345664"/>
+        <c:axId val="167627008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -880,12 +776,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="29347840"/>
+        <c:crossAx val="167776640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="29347840"/>
+        <c:axId val="167776640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -921,7 +817,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="29345664"/>
+        <c:crossAx val="167627008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1556,80 +1452,74 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:11" ht="15" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:11" ht="15" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F3">
-        <f>E3+1</f>
+        <v>6</v>
+      </c>
+      <c r="G3">
+        <v>5</v>
+      </c>
+      <c r="H3">
+        <v>4</v>
+      </c>
+      <c r="I3">
+        <v>3</v>
+      </c>
+      <c r="J3">
+        <v>2</v>
+      </c>
+      <c r="K3">
         <v>1</v>
       </c>
-      <c r="G3">
-        <f t="shared" ref="G3:K3" si="0">F3+1</f>
-        <v>2</v>
-      </c>
-      <c r="H3">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="I3">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="J3">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="K3">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:11" ht="15" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
         <v>2</v>
       </c>
       <c r="E4">
         <f>E3*0.2</f>
-        <v>0</v>
+        <v>1.2000000000000002</v>
       </c>
       <c r="F4">
-        <f t="shared" ref="F4:K4" si="1">F3*0.2</f>
+        <f t="shared" ref="F4:K4" si="0">F3*0.2</f>
+        <v>1.2000000000000002</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="0"/>
+        <v>0.8</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="0"/>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="0"/>
+        <v>0.4</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="0"/>
         <v>0.2</v>
-      </c>
-      <c r="G4">
-        <f t="shared" si="1"/>
-        <v>0.4</v>
-      </c>
-      <c r="H4">
-        <f t="shared" si="1"/>
-        <v>0.60000000000000009</v>
-      </c>
-      <c r="I4">
-        <f t="shared" si="1"/>
-        <v>0.8</v>
-      </c>
-      <c r="J4">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="K4">
-        <f t="shared" si="1"/>
-        <v>1.2000000000000002</v>
       </c>
     </row>
     <row r="5" spans="2:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1638,39 +1528,39 @@
       </c>
       <c r="E5">
         <f>EXP(-0.45*E3)</f>
-        <v>1</v>
+        <v>6.7205512739749756E-2</v>
       </c>
       <c r="F5">
         <f>1-EXP(-0.45*F3)</f>
+        <v>0.93279448726025027</v>
+      </c>
+      <c r="G5">
+        <f t="shared" ref="G5:K5" si="1">1-EXP(-0.45*G3)</f>
+        <v>0.89460077543813565</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="1"/>
+        <v>0.83470111177841344</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="1"/>
+        <v>0.74075973935410855</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="1"/>
+        <v>0.59343034025940089</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="1"/>
         <v>0.36237184837822667</v>
       </c>
-      <c r="G5">
-        <f t="shared" ref="G5:K5" si="2">1-EXP(-0.45*G3)</f>
-        <v>0.59343034025940089</v>
-      </c>
-      <c r="H5">
-        <f t="shared" si="2"/>
-        <v>0.74075973935410855</v>
-      </c>
-      <c r="I5">
-        <f t="shared" si="2"/>
-        <v>0.83470111177841344</v>
-      </c>
-      <c r="J5">
-        <f t="shared" si="2"/>
-        <v>0.89460077543813565</v>
-      </c>
-      <c r="K5">
-        <f t="shared" si="2"/>
-        <v>0.93279448726025027</v>
-      </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:11" ht="15" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:11" ht="15" x14ac:dyDescent="0.25">
       <c r="D7">
         <v>0</v>
       </c>
@@ -1682,432 +1572,432 @@
         <v>0</v>
       </c>
       <c r="G7">
-        <f t="shared" ref="G7:K7" si="3">G$4*(1-EXP(-G$5*$D7/G$4))</f>
+        <f t="shared" ref="G7:K7" si="2">G$4*(1-EXP(-G$5*$D7/G$4))</f>
         <v>0</v>
       </c>
       <c r="H7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:11" ht="15" x14ac:dyDescent="0.25">
       <c r="D8">
         <f>D7+0.5</f>
         <v>0.5</v>
       </c>
       <c r="E8">
-        <f t="shared" ref="E8:E19" si="4">E$4*(1-EXP(-$E$5*E$4/$D8))</f>
-        <v>0</v>
+        <f t="shared" ref="E8:E19" si="3">E$4*(1-EXP(-$E$5*E$4/$D8))</f>
+        <v>0.17874902059373804</v>
       </c>
       <c r="F8">
-        <f t="shared" ref="F8:K19" si="5">F$4*(1-EXP(-F$5*$D8/F$4))</f>
+        <f t="shared" ref="F8:K19" si="4">F$4*(1-EXP(-F$5*$D8/F$4))</f>
+        <v>0.38644586837665329</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="4"/>
+        <v>0.36064817401002547</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="4"/>
+        <v>0.32518581747851849</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="4"/>
+        <v>0.27636061961420105</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="4"/>
+        <v>0.20949534655833113</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="4"/>
         <v>0.11916680215186558</v>
       </c>
-      <c r="G8">
+    </row>
+    <row r="9" spans="2:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <f t="shared" ref="D9:D19" si="5">D8+0.5</f>
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="3"/>
+        <v>9.2976434176979969E-2</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="4"/>
+        <v>0.6484413957654851</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="4"/>
+        <v>0.59122924260328524</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="4"/>
+        <v>0.51818936509557145</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="4"/>
+        <v>0.4254292524391603</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="4"/>
+        <v>0.30926994254267415</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="4"/>
+        <v>0.16732997062822177</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="D10">
         <f t="shared" si="5"/>
-        <v>0.20949534655833113</v>
-      </c>
-      <c r="H8">
+        <v>1.5</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="3"/>
+        <v>6.2813594226516903E-2</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="4"/>
+        <v>0.82606434891050351</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="4"/>
+        <v>0.73865166984710562</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="4"/>
+        <v>0.63274039220249267</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="4"/>
+        <v>0.50583671904320682</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="4"/>
+        <v>0.35678875461837362</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="4"/>
+        <v>0.18679588526043345</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="D11">
         <f t="shared" si="5"/>
-        <v>0.27636061961420105</v>
-      </c>
-      <c r="I8">
+        <v>2</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="3"/>
+        <v>4.7425369449932794E-2</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="4"/>
+        <v>0.94648592174572821</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="4"/>
+        <v>0.83290646789731626</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="4"/>
+        <v>0.7007284575684537</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="4"/>
+        <v>0.54920842349341603</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="4"/>
+        <v>0.37942014168447585</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="4"/>
+        <v>0.19466334590423576</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="D12">
         <f t="shared" si="5"/>
-        <v>0.32518581747851849</v>
-      </c>
-      <c r="J8">
+        <v>2.5</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="3"/>
+        <v>3.8092663191591929E-2</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="4"/>
+        <v>1.0281271451762939</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="4"/>
+        <v>0.89316844513903471</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="4"/>
+        <v>0.74108057966589846</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="4"/>
+        <v>0.57260307608431882</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="4"/>
+        <v>0.39019860305930609</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="4"/>
+        <v>0.19784310591815016</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="D13">
         <f t="shared" si="5"/>
-        <v>0.36064817401002547</v>
-      </c>
-      <c r="K8">
+        <v>3</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="3"/>
+        <v>3.1828913673951714E-2</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="4"/>
+        <v>1.0834767740368954</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="4"/>
+        <v>0.93169705032629369</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="4"/>
+        <v>0.76503027949928004</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="4"/>
+        <v>0.5852221275324202</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="4"/>
+        <v>0.39533197068142223</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="4"/>
+        <v>0.19912825676972182</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="D14">
         <f t="shared" si="5"/>
-        <v>0.38644586837665329</v>
+        <v>3.5</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="3"/>
+        <v>2.7334143570085439E-2</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="4"/>
+        <v>1.1210017067396962</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="4"/>
+        <v>0.95633038440561458</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="4"/>
+        <v>0.77924485093430751</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="4"/>
+        <v>0.59202883085195357</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="4"/>
+        <v>0.39777679673102195</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="4"/>
+        <v>0.19964767103497078</v>
       </c>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="D9">
-        <f t="shared" ref="D9:D19" si="6">D8+0.5</f>
-        <v>1</v>
-      </c>
-      <c r="E9">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="F9">
+    <row r="15" spans="2:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="D15">
         <f t="shared" si="5"/>
-        <v>0.16732997062822177</v>
-      </c>
-      <c r="G9">
-        <f t="shared" si="5"/>
-        <v>0.30926994254267415</v>
-      </c>
-      <c r="H9">
-        <f t="shared" si="5"/>
-        <v>0.4254292524391603</v>
-      </c>
-      <c r="I9">
-        <f t="shared" si="5"/>
-        <v>0.51818936509557145</v>
-      </c>
-      <c r="J9">
-        <f t="shared" si="5"/>
-        <v>0.59122924260328524</v>
-      </c>
-      <c r="K9">
-        <f t="shared" si="5"/>
-        <v>0.6484413957654851</v>
+        <v>4</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="3"/>
+        <v>2.3951720098158272E-2</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="4"/>
+        <v>1.1464421767724058</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="4"/>
+        <v>0.97207975152944937</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="4"/>
+        <v>0.78768145107907717</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="4"/>
+        <v>0.59570035959329315</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="4"/>
+        <v>0.39894117357928238</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="4"/>
+        <v>0.19985760061531083</v>
       </c>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="D10">
-        <f t="shared" si="6"/>
-        <v>1.5</v>
-      </c>
-      <c r="E10">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <f t="shared" si="5"/>
-        <v>0.18679588526043345</v>
-      </c>
-      <c r="G10">
-        <f t="shared" si="5"/>
-        <v>0.35678875461837362</v>
-      </c>
-      <c r="H10">
-        <f t="shared" si="5"/>
-        <v>0.50583671904320682</v>
-      </c>
-      <c r="I10">
-        <f t="shared" si="5"/>
-        <v>0.63274039220249267</v>
-      </c>
-      <c r="J10">
-        <f t="shared" si="5"/>
-        <v>0.73865166984710562</v>
-      </c>
-      <c r="K10">
-        <f t="shared" si="5"/>
-        <v>0.82606434891050351</v>
-      </c>
-    </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="D11">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="E11">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="F11">
-        <f t="shared" si="5"/>
-        <v>0.19466334590423576</v>
-      </c>
-      <c r="G11">
-        <f t="shared" si="5"/>
-        <v>0.37942014168447585</v>
-      </c>
-      <c r="H11">
-        <f t="shared" si="5"/>
-        <v>0.54920842349341603</v>
-      </c>
-      <c r="I11">
-        <f t="shared" si="5"/>
-        <v>0.7007284575684537</v>
-      </c>
-      <c r="J11">
-        <f t="shared" si="5"/>
-        <v>0.83290646789731626</v>
-      </c>
-      <c r="K11">
-        <f t="shared" si="5"/>
-        <v>0.94648592174572821</v>
-      </c>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="D12">
-        <f t="shared" si="6"/>
-        <v>2.5</v>
-      </c>
-      <c r="E12">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="F12">
-        <f t="shared" si="5"/>
-        <v>0.19784310591815016</v>
-      </c>
-      <c r="G12">
-        <f t="shared" si="5"/>
-        <v>0.39019860305930609</v>
-      </c>
-      <c r="H12">
-        <f t="shared" si="5"/>
-        <v>0.57260307608431882</v>
-      </c>
-      <c r="I12">
-        <f t="shared" si="5"/>
-        <v>0.74108057966589846</v>
-      </c>
-      <c r="J12">
-        <f t="shared" si="5"/>
-        <v>0.89316844513903471</v>
-      </c>
-      <c r="K12">
-        <f t="shared" si="5"/>
-        <v>1.0281271451762939</v>
-      </c>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="D13">
-        <f t="shared" si="6"/>
-        <v>3</v>
-      </c>
-      <c r="E13">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="F13">
-        <f t="shared" si="5"/>
-        <v>0.19912825676972182</v>
-      </c>
-      <c r="G13">
-        <f t="shared" si="5"/>
-        <v>0.39533197068142223</v>
-      </c>
-      <c r="H13">
-        <f t="shared" si="5"/>
-        <v>0.5852221275324202</v>
-      </c>
-      <c r="I13">
-        <f t="shared" si="5"/>
-        <v>0.76503027949928004</v>
-      </c>
-      <c r="J13">
-        <f t="shared" si="5"/>
-        <v>0.93169705032629369</v>
-      </c>
-      <c r="K13">
-        <f t="shared" si="5"/>
-        <v>1.0834767740368954</v>
-      </c>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="D14">
-        <f t="shared" si="6"/>
-        <v>3.5</v>
-      </c>
-      <c r="E14">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="F14">
-        <f t="shared" si="5"/>
-        <v>0.19964767103497078</v>
-      </c>
-      <c r="G14">
-        <f t="shared" si="5"/>
-        <v>0.39777679673102195</v>
-      </c>
-      <c r="H14">
-        <f t="shared" si="5"/>
-        <v>0.59202883085195357</v>
-      </c>
-      <c r="I14">
-        <f t="shared" si="5"/>
-        <v>0.77924485093430751</v>
-      </c>
-      <c r="J14">
-        <f t="shared" si="5"/>
-        <v>0.95633038440561458</v>
-      </c>
-      <c r="K14">
-        <f t="shared" si="5"/>
-        <v>1.1210017067396962</v>
-      </c>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="D15">
-        <f t="shared" si="6"/>
-        <v>4</v>
-      </c>
-      <c r="E15">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="F15">
-        <f t="shared" si="5"/>
-        <v>0.19985760061531083</v>
-      </c>
-      <c r="G15">
-        <f t="shared" si="5"/>
-        <v>0.39894117357928238</v>
-      </c>
-      <c r="H15">
-        <f t="shared" si="5"/>
-        <v>0.59570035959329315</v>
-      </c>
-      <c r="I15">
-        <f t="shared" si="5"/>
-        <v>0.78768145107907717</v>
-      </c>
-      <c r="J15">
-        <f t="shared" si="5"/>
-        <v>0.97207975152944937</v>
-      </c>
-      <c r="K15">
-        <f t="shared" si="5"/>
-        <v>1.1464421767724058</v>
-      </c>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:11" ht="15" x14ac:dyDescent="0.25">
       <c r="D16">
         <f>D15+0.5</f>
         <v>4.5</v>
       </c>
       <c r="E16">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>2.1314202684086729E-2</v>
       </c>
       <c r="F16">
+        <f t="shared" si="4"/>
+        <v>1.1636898430270317</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="4"/>
+        <v>0.98214913815825966</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="4"/>
+        <v>0.79268872283032643</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="4"/>
+        <v>0.59768077840481937</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="4"/>
+        <v>0.3994957215991658</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="4"/>
+        <v>0.19994244701181985</v>
+      </c>
+    </row>
+    <row r="17" spans="4:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="D17">
         <f t="shared" si="5"/>
-        <v>0.19994244701181985</v>
-      </c>
-      <c r="G16">
+        <v>5</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="3"/>
+        <v>1.9199930483534501E-2</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="4"/>
+        <v>1.175383101478958</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="4"/>
+        <v>0.98858701888598854</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="4"/>
+        <v>0.79566062738436694</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="4"/>
+        <v>0.59874901426659743</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="4"/>
+        <v>0.39975983154502742</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="4"/>
+        <v>0.19997673903959842</v>
+      </c>
+    </row>
+    <row r="18" spans="4:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="D18">
         <f t="shared" si="5"/>
-        <v>0.3994957215991658</v>
-      </c>
-      <c r="H16">
+        <v>5.5</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="3"/>
+        <v>1.7467250861043528E-2</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="4"/>
+        <v>1.183310683750378</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="4"/>
+        <v>0.99270308968476773</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="4"/>
+        <v>0.79742450542356513</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="4"/>
+        <v>0.59932521958728358</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="4"/>
+        <v>0.39988561697929459</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="4"/>
+        <v>0.19999059871092861</v>
+      </c>
+    </row>
+    <row r="19" spans="4:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="D19">
         <f t="shared" si="5"/>
-        <v>0.59768077840481937</v>
-      </c>
-      <c r="I16">
-        <f t="shared" si="5"/>
-        <v>0.79268872283032643</v>
-      </c>
-      <c r="J16">
-        <f t="shared" si="5"/>
-        <v>0.98214913815825966</v>
-      </c>
-      <c r="K16">
-        <f t="shared" si="5"/>
-        <v>1.1636898430270317</v>
-      </c>
-    </row>
-    <row r="17" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D17">
-        <f t="shared" si="6"/>
-        <v>5</v>
-      </c>
-      <c r="E17">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="F17">
-        <f t="shared" si="5"/>
-        <v>0.19997673903959842</v>
-      </c>
-      <c r="G17">
-        <f t="shared" si="5"/>
-        <v>0.39975983154502742</v>
-      </c>
-      <c r="H17">
-        <f t="shared" si="5"/>
-        <v>0.59874901426659743</v>
-      </c>
-      <c r="I17">
-        <f t="shared" si="5"/>
-        <v>0.79566062738436694</v>
-      </c>
-      <c r="J17">
-        <f t="shared" si="5"/>
-        <v>0.98858701888598854</v>
-      </c>
-      <c r="K17">
-        <f t="shared" si="5"/>
-        <v>1.175383101478958</v>
-      </c>
-    </row>
-    <row r="18" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D18">
-        <f t="shared" si="6"/>
-        <v>5.5</v>
-      </c>
-      <c r="E18">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="F18">
-        <f t="shared" si="5"/>
-        <v>0.19999059871092861</v>
-      </c>
-      <c r="G18">
-        <f t="shared" si="5"/>
-        <v>0.39988561697929459</v>
-      </c>
-      <c r="H18">
-        <f t="shared" si="5"/>
-        <v>0.59932521958728358</v>
-      </c>
-      <c r="I18">
-        <f t="shared" si="5"/>
-        <v>0.79742450542356513</v>
-      </c>
-      <c r="J18">
-        <f t="shared" si="5"/>
-        <v>0.99270308968476773</v>
-      </c>
-      <c r="K18">
-        <f t="shared" si="5"/>
-        <v>1.183310683750378</v>
-      </c>
-    </row>
-    <row r="19" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D19">
-        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="E19">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1.6021409149955094E-2</v>
       </c>
       <c r="F19">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
+        <v>1.1886852815092928</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="4"/>
+        <v>0.99533470706587113</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="4"/>
+        <v>0.79847139831012692</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="4"/>
+        <v>0.59963602414221995</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="4"/>
+        <v>0.39994552375570225</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="4"/>
         <v>0.19999620031870233</v>
-      </c>
-      <c r="G19">
-        <f t="shared" si="5"/>
-        <v>0.39994552375570225</v>
-      </c>
-      <c r="H19">
-        <f t="shared" si="5"/>
-        <v>0.59963602414221995</v>
-      </c>
-      <c r="I19">
-        <f t="shared" si="5"/>
-        <v>0.79847139831012692</v>
-      </c>
-      <c r="J19">
-        <f t="shared" si="5"/>
-        <v>0.99533470706587113</v>
-      </c>
-      <c r="K19">
-        <f t="shared" si="5"/>
-        <v>1.1886852815092928</v>
       </c>
     </row>
   </sheetData>
@@ -2122,7 +2012,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2134,7 +2024,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>